<commit_message>
[LC-568] Generate output file for generic messages [LC-676] Coordination output file: refactoring and unit tests
Signed-off-by: OUESLATI Wyem Ext <wyem.oueslati@rte-france.com>
</commit_message>
<xml_diff>
--- a/letsco-api/src/test/resources/validTestFileWithLowercaseTitles.xlsx
+++ b/letsco-api/src/test/resources/validTestFileWithLowercaseTitles.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="148">
   <si>
     <t xml:space="preserve">verb</t>
   </si>
@@ -81,6 +81,9 @@
     <t xml:space="preserve">businessapplication</t>
   </si>
   <si>
+    <t xml:space="preserve">recipients</t>
+  </si>
+  <si>
     <t xml:space="preserve">created</t>
   </si>
   <si>
@@ -121,6 +124,9 @@
   </si>
   <si>
     <t xml:space="preserve">PanEuropeanServiceATool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10XFR-RTE------Q;10X1001A1001A345</t>
   </si>
   <si>
     <t xml:space="preserve">datatype</t>
@@ -1081,10 +1087,10 @@
   </sheetPr>
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1106,7 +1112,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="32.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="19.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="28.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="33.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="1" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="24.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="19.42"/>
@@ -1171,62 +1177,68 @@
       <c r="R1" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="Y1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G2" s="8" t="n">
         <v>101</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M2" s="8" t="n">
         <v>24</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="9" t="s">
-        <v>29</v>
-      </c>
       <c r="Q2" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="Y2" s="0"/>
     </row>
@@ -1251,28 +1263,28 @@
     </row>
     <row r="4" s="21" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="17"/>
@@ -1295,10 +1307,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -1306,7 +1318,7 @@
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
       <c r="H5" s="24" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J5" s="17"/>
       <c r="K5" s="17"/>
@@ -1328,10 +1340,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="26" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -1339,7 +1351,7 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="27" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J6" s="17"/>
       <c r="K6" s="17"/>
@@ -1361,20 +1373,20 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
@@ -1396,20 +1408,20 @@
     </row>
     <row r="8" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="26" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="30" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
@@ -1431,20 +1443,20 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="26" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="31" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
@@ -1466,20 +1478,20 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="23" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="33" t="n">
@@ -1505,23 +1517,23 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="26" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="34" t="s">
-        <v>57</v>
-      </c>
       <c r="G11" s="34" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H11" s="27" t="n">
         <v>1</v>
@@ -1546,23 +1558,23 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="26" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="34" t="s">
-        <v>57</v>
-      </c>
       <c r="G12" s="34" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H12" s="27" t="n">
         <v>0</v>
@@ -1587,23 +1599,23 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="26" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H13" s="27" t="n">
         <v>1</v>
@@ -1628,23 +1640,23 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="26" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F14" s="34" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H14" s="27" t="n">
         <v>1</v>
@@ -1669,16 +1681,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
       <c r="F15" s="32" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G15" s="35"/>
       <c r="H15" s="33" t="n">
@@ -1704,16 +1716,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="26" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G16" s="36"/>
       <c r="H16" s="27" t="n">
@@ -1739,58 +1751,58 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C17" s="35"/>
       <c r="D17" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E17" s="23"/>
       <c r="F17" s="32" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G17" s="37"/>
       <c r="H17" s="38" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="26" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C18" s="36"/>
       <c r="D18" s="17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="34" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G18" s="39"/>
       <c r="H18" s="40" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="26" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C19" s="36"/>
       <c r="D19" s="36" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E19" s="36"/>
       <c r="F19" s="34" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G19" s="39"/>
       <c r="H19" s="40" t="n">
@@ -1799,58 +1811,58 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="26" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C20" s="36"/>
       <c r="D20" s="17" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G20" s="39"/>
       <c r="H20" s="40" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="26" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C21" s="36"/>
       <c r="D21" s="17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G21" s="39"/>
       <c r="H21" s="40" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="26" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C22" s="36"/>
       <c r="D22" s="36" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E22" s="36"/>
       <c r="F22" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G22" s="39"/>
       <c r="H22" s="40" t="n">
@@ -1859,44 +1871,44 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C23" s="35" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E23" s="23"/>
       <c r="F23" s="32" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H23" s="38" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="26" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C24" s="36" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="36" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E24" s="36"/>
       <c r="F24" s="34" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G24" s="39"/>
       <c r="H24" s="40" t="n">
@@ -1905,69 +1917,69 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="26" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C25" s="36" t="n">
         <v>2</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="34" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H25" s="40" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="26" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C26" s="36" t="n">
         <v>2</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="34" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H26" s="40" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="41" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C27" s="42"/>
       <c r="D27" s="42" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E27" s="42"/>
       <c r="F27" s="43" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G27" s="44" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H27" s="45" t="n">
         <f aca="false">RANDBETWEEN(1000,6000)</f>
@@ -1976,21 +1988,21 @@
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="46" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B28" s="47" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E28" s="47"/>
       <c r="F28" s="48" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G28" s="49" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H28" s="50" t="n">
         <f aca="false">RANDBETWEEN(1000,6000)</f>
@@ -1999,21 +2011,21 @@
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="46" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B29" s="47" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C29" s="47"/>
       <c r="D29" s="47" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E29" s="47"/>
       <c r="F29" s="48" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G29" s="49" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H29" s="50" t="n">
         <f aca="false">RANDBETWEEN(1000,6000)</f>
@@ -2022,21 +2034,21 @@
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="46" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B30" s="47" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C30" s="47"/>
       <c r="D30" s="47" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E30" s="47"/>
       <c r="F30" s="48" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G30" s="49" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H30" s="50" t="n">
         <f aca="false">RANDBETWEEN(1000,6000)</f>
@@ -2084,129 +2096,129 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="51" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F1" s="51" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="51" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H1" s="51" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C2" s="53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E2" s="53" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F2" s="53" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G2" s="53" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H2" s="53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B3" s="53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D3" s="53" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E3" s="53" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F3" s="53" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G3" s="53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H3" s="53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B4" s="53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C4" s="53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D4" s="53" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F4" s="53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G4" s="53" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H4" s="53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B5" s="53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F5" s="53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G5" s="53" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H5" s="53" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2259,31 +2271,31 @@
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="55" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D3" s="56" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F3" s="56" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G3" s="56" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H3" s="56" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I3" s="56" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J3" s="56" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2291,23 +2303,23 @@
         <v>1</v>
       </c>
       <c r="C4" s="55" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D4" s="57" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E4" s="57" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F4" s="55" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G4" s="58" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H4" s="59"/>
       <c r="I4" s="58" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J4" s="59"/>
     </row>
@@ -2318,11 +2330,11 @@
       <c r="E5" s="57"/>
       <c r="F5" s="55"/>
       <c r="G5" s="60" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H5" s="61"/>
       <c r="I5" s="60" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J5" s="61"/>
     </row>
@@ -2330,20 +2342,20 @@
       <c r="B6" s="55"/>
       <c r="C6" s="55"/>
       <c r="D6" s="62" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E6" s="62" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F6" s="55" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G6" s="60" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H6" s="61"/>
       <c r="I6" s="60" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J6" s="61"/>
     </row>
@@ -2354,11 +2366,11 @@
       <c r="E7" s="62"/>
       <c r="F7" s="55"/>
       <c r="G7" s="60" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H7" s="61"/>
       <c r="I7" s="60" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J7" s="61"/>
     </row>
@@ -2366,20 +2378,20 @@
       <c r="B8" s="55"/>
       <c r="C8" s="55"/>
       <c r="D8" s="63" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E8" s="63" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F8" s="55" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G8" s="60" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H8" s="61"/>
       <c r="I8" s="60" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J8" s="61"/>
     </row>
@@ -2391,32 +2403,32 @@
       <c r="F9" s="55"/>
       <c r="G9" s="61"/>
       <c r="H9" s="60" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I9" s="61"/>
       <c r="J9" s="60" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="55"/>
       <c r="C10" s="55"/>
       <c r="D10" s="64" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E10" s="64" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F10" s="55" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G10" s="61"/>
       <c r="H10" s="60" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I10" s="61"/>
       <c r="J10" s="60" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2427,32 +2439,32 @@
       <c r="F11" s="55"/>
       <c r="G11" s="61"/>
       <c r="H11" s="60" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I11" s="61"/>
       <c r="J11" s="60" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="55"/>
       <c r="C12" s="55"/>
       <c r="D12" s="65" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E12" s="65" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F12" s="55" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G12" s="61"/>
       <c r="H12" s="60" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I12" s="61"/>
       <c r="J12" s="60" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2463,33 +2475,33 @@
       <c r="F13" s="55"/>
       <c r="G13" s="61"/>
       <c r="H13" s="60" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="I13" s="61"/>
       <c r="J13" s="60" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="55"/>
       <c r="C14" s="55" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D14" s="57" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F14" s="55" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G14" s="60" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H14" s="61"/>
       <c r="I14" s="60" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J14" s="61"/>
     </row>
@@ -2500,11 +2512,11 @@
       <c r="E15" s="57"/>
       <c r="F15" s="55"/>
       <c r="G15" s="60" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H15" s="61"/>
       <c r="I15" s="60" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J15" s="61"/>
     </row>
@@ -2512,20 +2524,20 @@
       <c r="B16" s="55"/>
       <c r="C16" s="55"/>
       <c r="D16" s="62" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F16" s="55" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G16" s="60" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H16" s="61"/>
       <c r="I16" s="60" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J16" s="61"/>
     </row>
@@ -2536,11 +2548,11 @@
       <c r="E17" s="62"/>
       <c r="F17" s="55"/>
       <c r="G17" s="60" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H17" s="61"/>
       <c r="I17" s="60" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J17" s="61"/>
     </row>
@@ -2548,20 +2560,20 @@
       <c r="B18" s="55"/>
       <c r="C18" s="55"/>
       <c r="D18" s="63" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E18" s="63" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F18" s="55" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G18" s="60" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H18" s="61"/>
       <c r="I18" s="60" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J18" s="61"/>
     </row>
@@ -2573,32 +2585,32 @@
       <c r="F19" s="55"/>
       <c r="G19" s="61"/>
       <c r="H19" s="60" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I19" s="61"/>
       <c r="J19" s="60" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="55"/>
       <c r="C20" s="55"/>
       <c r="D20" s="64" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E20" s="64" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F20" s="55" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G20" s="61"/>
       <c r="H20" s="60" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I20" s="61"/>
       <c r="J20" s="60" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2609,32 +2621,32 @@
       <c r="F21" s="55"/>
       <c r="G21" s="61"/>
       <c r="H21" s="60" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I21" s="61"/>
       <c r="J21" s="60" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="55"/>
       <c r="C22" s="55"/>
       <c r="D22" s="65" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E22" s="65" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="F22" s="55" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G22" s="61"/>
       <c r="H22" s="60" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I22" s="61"/>
       <c r="J22" s="60" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2645,11 +2657,11 @@
       <c r="F23" s="55"/>
       <c r="G23" s="61"/>
       <c r="H23" s="60" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="I23" s="61"/>
       <c r="J23" s="60" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>